<commit_message>
actualuzación descripción de nuevos masivos y script datos BAU en EEE y EESI
</commit_message>
<xml_diff>
--- a/back-end/Web Dinamico 2/MRVMinem/Documentos/1.1 Plantilla_Etiquetado_de_eficiencia_Aire acondicionado.xlsx
+++ b/back-end/Web Dinamico 2/MRVMinem/Documentos/1.1 Plantilla_Etiquetado_de_eficiencia_Aire acondicionado.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Versión borrado de meses y fechas SOLO SE DEJO AÑOS _V2\Plantillas etiquetado nueva versión con desplegable ABCDEF\Pnatillas sin etiquetas desplegables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E37149-F884-4AA7-842F-A4ED9CDDF55C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370010E5-3549-4F19-85F1-8F93DF3BF1FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{0FF7017A-1C1F-4F31-834A-BE5FD5CEB108}"/>
   </bookViews>
@@ -163,9 +163,6 @@
     <t>Etiqueta de EE del equipo anterior o reemplazado. Seleccione de la lista desplegable.</t>
   </si>
   <si>
-    <t>Etiqueta de EE del equipo nuevo. Seleccione de la lista desplegable.</t>
-  </si>
-  <si>
     <t>9000 BTU/H</t>
   </si>
   <si>
@@ -188,6 +185,9 @@
   </si>
   <si>
     <t>Etiqueta de EE acción</t>
+  </si>
+  <si>
+    <t>Etiqueta de EE del equipo nuevo.</t>
   </si>
 </sst>
 </file>
@@ -882,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2029263-33DE-46C6-ADE8-A69CDB86AC1C}">
   <dimension ref="A1:T312"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,8 +904,10 @@
     <col min="14" max="14" width="15.7109375" customWidth="1"/>
     <col min="15" max="15" width="11.42578125" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="22.85546875" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" customWidth="1"/>
     <col min="18" max="18" width="11.42578125" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="22.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -934,7 +936,7 @@
         <v>4</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J1" s="9" t="s">
         <v>34</v>
@@ -952,19 +954,19 @@
         <v>4</v>
       </c>
       <c r="O1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>44</v>
       </c>
       <c r="Q1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="R1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>44</v>
       </c>
       <c r="T1" s="9" t="s">
         <v>4</v>
@@ -1007,32 +1009,32 @@
         <v>35</v>
       </c>
       <c r="F3" s="30"/>
-      <c r="G3" s="29" t="s">
-        <v>36</v>
+      <c r="G3" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>29</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="K3" s="13" t="s">
         <v>29</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="N3" s="13" t="s">
         <v>29</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="Q3" s="13" t="s">
         <v>29</v>
       </c>
       <c r="S3" s="13" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="T3" s="13" t="s">
         <v>29</v>
@@ -1047,7 +1049,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="14">
         <f t="shared" ref="D4:D67" si="1">VLOOKUP(E4,Tabla_BAU,2,)</f>
@@ -17426,7 +17428,7 @@
       <c r="T312" s="27"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="HNLCsNInq+Doi2ygc4uwde1syYyp44FWj4JMJDmbVbP/aDqCFTnaL/yxnTktCP0AoD4VoGPO3qS5HCiE+s/Vyw==" saltValue="abQvVLvYu6Xtgr8wac073A==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ZCweHM92hY4Umt2MkpRX9fy41Iy2yLDdOA1KnfEXld9pd6lg/cKlvZRTA8OvF/Oay6Ptrf22xGgmUFoOZkuH/A==" saltValue="amKp+9Qj+vLKavUmX8EDIQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="A2:T2"/>
   </mergeCells>
@@ -17534,7 +17536,7 @@
         <v>2013</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
@@ -17563,7 +17565,7 @@
         <v>2014</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="5">
         <v>2</v>
@@ -17592,7 +17594,7 @@
         <v>2015</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="5">
         <v>3</v>
@@ -17621,7 +17623,7 @@
         <v>2016</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="5">
         <v>4</v>
@@ -17650,7 +17652,7 @@
         <v>2017</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="5">
         <v>5</v>
@@ -17679,7 +17681,7 @@
         <v>2018</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="8">
         <v>6</v>

</xml_diff>

<commit_message>
Cambios en los masivos EEE y EESI plantilla segun nuevas descripciones
</commit_message>
<xml_diff>
--- a/back-end/Web Dinamico 2/MRVMinem/Documentos/1.1 Plantilla_Etiquetado_de_eficiencia_Aire acondicionado.xlsx
+++ b/back-end/Web Dinamico 2/MRVMinem/Documentos/1.1 Plantilla_Etiquetado_de_eficiencia_Aire acondicionado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Versión borrado de meses y fechas SOLO SE DEJO AÑOS _V2\Plantillas etiquetado nueva versión con desplegable ABCDEF\Pnatillas sin etiquetas desplegables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370010E5-3549-4F19-85F1-8F93DF3BF1FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2198A6B9-82A9-406D-A125-82E5669B2B19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{0FF7017A-1C1F-4F31-834A-BE5FD5CEB108}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="56">
   <si>
     <t>Año</t>
   </si>
@@ -142,25 +142,10 @@
     <t>Diciembre</t>
   </si>
   <si>
-    <t>Número de unidades de este equipo. Inserte su dato.</t>
-  </si>
-  <si>
-    <t>Año en que se compró el equipo. Seleccione de la lista desplegable.</t>
-  </si>
-  <si>
-    <t>Capacidad del  aire acondicionado. Seleccione de la lista desplegable.</t>
-  </si>
-  <si>
     <t>Registrar sus datos según el ejemplo brindado. Borre estos datos y complete los suyos.</t>
   </si>
   <si>
     <t>Etiqueta de EE BAU</t>
-  </si>
-  <si>
-    <t>Etiqueta de EE Acción</t>
-  </si>
-  <si>
-    <t>Etiqueta de EE del equipo anterior o reemplazado. Seleccione de la lista desplegable.</t>
   </si>
   <si>
     <t>9000 BTU/H</t>
@@ -184,10 +169,58 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Etiqueta de EE acción</t>
+    <t>Año de registro. Seleccione de la lista desplegable.</t>
   </si>
   <si>
-    <t>Etiqueta de EE del equipo nuevo.</t>
+    <t>Capacidad del equipo  aire acondicionado. Seleccione de la lista desplegable.</t>
+  </si>
+  <si>
+    <t>Etiqueta de EE de linea base. Seleccione de la lista desplegable.</t>
+  </si>
+  <si>
+    <t>Etiqueta de EE (A)</t>
+  </si>
+  <si>
+    <t>Etiqueta de EE (B)</t>
+  </si>
+  <si>
+    <t>Etiqueta de EE (C)</t>
+  </si>
+  <si>
+    <t>Etiqueta de EE (D)</t>
+  </si>
+  <si>
+    <t>Etiqueta de eficiencia energética tipo A.</t>
+  </si>
+  <si>
+    <t>Número de equipos de aire acondicionado con la etiqueta A. En caso no se cuente con equipos de esta etiqueta colocar cero (0). Inserte su dato.</t>
+  </si>
+  <si>
+    <t>Etiqueta de EE (E)</t>
+  </si>
+  <si>
+    <t>Etiqueta de eficiencia energética tipo B.</t>
+  </si>
+  <si>
+    <t>Número de equipos de aire acondicionado con la etiqueta B. En caso no se cuente con equipos de esta etiqueta colocar cero (0). Inserte su dato.</t>
+  </si>
+  <si>
+    <t>Etiqueta de eficiencia energética tipo C.</t>
+  </si>
+  <si>
+    <t>Número de equipos de aire acondicionado con la etiqueta C. En caso no se cuente con equipos de esta etiqueta colocar cero (0). Inserte su dato.</t>
+  </si>
+  <si>
+    <t>Etiqueta de eficiencia energética tipo D.</t>
+  </si>
+  <si>
+    <t>Número de equipos de aire acondicionado con la etiqueta D. En caso no se cuente con equipos de esta etiqueta colocar cero (0). Inserte su dato.</t>
+  </si>
+  <si>
+    <t>Etiqueta de eficiencia energética tipo E.</t>
+  </si>
+  <si>
+    <t>Número de equipos de aire acondicionado con la etiqueta E. En caso no se cuente con equipos de esta etiqueta colocar cero (0). Inserte su dato.</t>
   </si>
 </sst>
 </file>
@@ -452,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -542,9 +575,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -882,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2029263-33DE-46C6-ADE8-A69CDB86AC1C}">
   <dimension ref="A1:T312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,20 +924,20 @@
     <col min="4" max="4" width="10.85546875" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="28.28515625" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="8" max="8" width="34.140625" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="26.85546875" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" customWidth="1"/>
+    <col min="11" max="11" width="35.42578125" customWidth="1"/>
     <col min="12" max="12" width="11.42578125" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="24.28515625" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" customWidth="1"/>
+    <col min="14" max="14" width="32.7109375" customWidth="1"/>
     <col min="15" max="15" width="11.42578125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="22.85546875" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" customWidth="1"/>
+    <col min="16" max="16" width="23" customWidth="1"/>
+    <col min="17" max="17" width="34.5703125" customWidth="1"/>
     <col min="18" max="18" width="11.42578125" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="22.28515625" customWidth="1"/>
-    <col min="20" max="20" width="13.5703125" customWidth="1"/>
+    <col min="20" max="20" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -924,22 +954,22 @@
         <v>1</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="H1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>34</v>
       </c>
       <c r="K1" s="9" t="s">
         <v>4</v>
@@ -948,96 +978,96 @@
         <v>1</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="N1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Q1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="S1" s="9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="T1" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-    </row>
-    <row r="3" spans="1:20" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+    </row>
+    <row r="3" spans="1:20" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="11" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D3" s="12"/>
-      <c r="E3" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="30"/>
+      <c r="E3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="29"/>
       <c r="G3" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="K3" s="13" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="Q3" s="13" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="S3" s="13" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="T3" s="13" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -1049,7 +1079,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D4" s="14">
         <f t="shared" ref="D4:D67" si="1">VLOOKUP(E4,Tabla_BAU,2,)</f>
@@ -1068,7 +1098,7 @@
       <c r="H4" s="15">
         <v>500</v>
       </c>
-      <c r="I4" s="34">
+      <c r="I4" s="33">
         <f t="shared" ref="I4:I67" si="3">VLOOKUP(J4,Tabla_BAU2,2,)</f>
         <v>1</v>
       </c>
@@ -1121,43 +1151,43 @@
         <v>#N/A</v>
       </c>
       <c r="E5" s="17"/>
-      <c r="F5" s="31">
+      <c r="F5" s="30">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="31" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="23"/>
-      <c r="I5" s="33">
+      <c r="I5" s="32">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="J5" s="32" t="s">
+      <c r="J5" s="31" t="s">
         <v>11</v>
       </c>
       <c r="K5" s="26"/>
-      <c r="L5" s="31">
+      <c r="L5" s="30">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="M5" s="32" t="s">
+      <c r="M5" s="31" t="s">
         <v>12</v>
       </c>
       <c r="N5" s="26"/>
-      <c r="O5" s="31">
+      <c r="O5" s="30">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="P5" s="32" t="s">
+      <c r="P5" s="31" t="s">
         <v>13</v>
       </c>
       <c r="Q5" s="26"/>
-      <c r="R5" s="31">
+      <c r="R5" s="30">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="S5" s="32" t="s">
+      <c r="S5" s="31" t="s">
         <v>14</v>
       </c>
       <c r="T5" s="26"/>
@@ -17428,7 +17458,7 @@
       <c r="T312" s="27"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ZCweHM92hY4Umt2MkpRX9fy41Iy2yLDdOA1KnfEXld9pd6lg/cKlvZRTA8OvF/Oay6Ptrf22xGgmUFoOZkuH/A==" saltValue="amKp+9Qj+vLKavUmX8EDIQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="WohFFV2pl//916HbLgNTzv7Ona/D1Z94KEIqpUtRxMplc6uCexq13CdhO3W8KHd7Q9nIe4o++YMqxNzObZyUDQ==" saltValue="EvOd492c4DI7PxoV4KNJDA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="A2:T2"/>
   </mergeCells>
@@ -17536,7 +17566,7 @@
         <v>2013</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
@@ -17565,7 +17595,7 @@
         <v>2014</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D9" s="5">
         <v>2</v>
@@ -17594,7 +17624,7 @@
         <v>2015</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D10" s="5">
         <v>3</v>
@@ -17623,7 +17653,7 @@
         <v>2016</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D11" s="5">
         <v>4</v>
@@ -17652,7 +17682,7 @@
         <v>2017</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D12" s="5">
         <v>5</v>
@@ -17681,7 +17711,7 @@
         <v>2018</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D13" s="8">
         <v>6</v>

</xml_diff>

<commit_message>
update de masivo EEE y EESI motores con textos evitar borrar
</commit_message>
<xml_diff>
--- a/back-end/Web Dinamico 2/MRVMinem/Documentos/1.1 Plantilla_Etiquetado_de_eficiencia_Aire acondicionado.xlsx
+++ b/back-end/Web Dinamico 2/MRVMinem/Documentos/1.1 Plantilla_Etiquetado_de_eficiencia_Aire acondicionado.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Versión borrado de meses y fechas SOLO SE DEJO AÑOS _V2\Plantillas etiquetado nueva versión con desplegable ABCDEF\Pnatillas sin etiquetas desplegables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Web Dinamico 2\MRVMinem\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2198A6B9-82A9-406D-A125-82E5669B2B19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9B63AA-DE32-4A0E-8008-DE4AA6BCCEE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{0FF7017A-1C1F-4F31-834A-BE5FD5CEB108}"/>
   </bookViews>
@@ -41,12 +41,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -142,9 +136,6 @@
     <t>Diciembre</t>
   </si>
   <si>
-    <t>Registrar sus datos según el ejemplo brindado. Borre estos datos y complete los suyos.</t>
-  </si>
-  <si>
     <t>Etiqueta de EE BAU</t>
   </si>
   <si>
@@ -221,6 +212,9 @@
   </si>
   <si>
     <t>Número de equipos de aire acondicionado con la etiqueta E. En caso no se cuente con equipos de esta etiqueta colocar cero (0). Inserte su dato.</t>
+  </si>
+  <si>
+    <t>Registrar sus datos según el ejemplo brindado. Borre estos datos y complete los suyos. Evite borrar las etiquetas que se muestran por defecto desplegadas.</t>
   </si>
 </sst>
 </file>
@@ -913,7 +907,7 @@
   <dimension ref="A1:T312"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,22 +948,22 @@
         <v>1</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K1" s="9" t="s">
         <v>4</v>
@@ -978,25 +972,25 @@
         <v>1</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S1" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T1" s="9" t="s">
         <v>4</v>
@@ -1004,7 +998,7 @@
     </row>
     <row r="2" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>
@@ -1028,46 +1022,46 @@
     </row>
     <row r="3" spans="1:20" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3" s="29"/>
       <c r="G3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="13" t="s">
-        <v>46</v>
-      </c>
       <c r="J3" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="M3" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="N3" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="N3" s="13" t="s">
+      <c r="P3" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="Q3" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="S3" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="S3" s="13" t="s">
+      <c r="T3" s="13" t="s">
         <v>54</v>
-      </c>
-      <c r="T3" s="13" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -1079,7 +1073,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="14">
         <f t="shared" ref="D4:D67" si="1">VLOOKUP(E4,Tabla_BAU,2,)</f>
@@ -17458,7 +17452,7 @@
       <c r="T312" s="27"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="WohFFV2pl//916HbLgNTzv7Ona/D1Z94KEIqpUtRxMplc6uCexq13CdhO3W8KHd7Q9nIe4o++YMqxNzObZyUDQ==" saltValue="EvOd492c4DI7PxoV4KNJDA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="1chQZLpoDUpCv6RIBefvQfWKKYRN3aYBho96FS9QONR8Og3IIznyzdPeZBBdMvgovTQ1FontcJjAYsVPsxCLvw==" saltValue="abh96JPT+it1CVNW5iyuIA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="A2:T2"/>
   </mergeCells>
@@ -17566,7 +17560,7 @@
         <v>2013</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
@@ -17595,7 +17589,7 @@
         <v>2014</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="5">
         <v>2</v>
@@ -17624,7 +17618,7 @@
         <v>2015</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="5">
         <v>3</v>
@@ -17653,7 +17647,7 @@
         <v>2016</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="5">
         <v>4</v>
@@ -17682,7 +17676,7 @@
         <v>2017</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="5">
         <v>5</v>
@@ -17711,7 +17705,7 @@
         <v>2018</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="8">
         <v>6</v>

</xml_diff>